<commit_message>
july, august excel files updated
</commit_message>
<xml_diff>
--- a/excelParsing/data/august_report.xlsx
+++ b/excelParsing/data/august_report.xlsx
@@ -16,25 +16,25 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="H2">
+    <comment authorId="0" ref="K2">
       <text>
         <t xml:space="preserve">added updated document name
 	-Madhurima Nath</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2">
+    <comment authorId="0" ref="J2">
       <text>
         <t xml:space="preserve">provided updated effective date
 	-Madhurima Nath</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D4">
+    <comment authorId="0" ref="G4">
       <text>
         <t xml:space="preserve">provided updated link
 	-Madhurima Nath</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B4">
+    <comment authorId="0" ref="E4">
       <text>
         <t xml:space="preserve">provided updated date
 	-Madhurima Nath</t>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Country</t>
   </si>
@@ -68,12 +68,15 @@
     <t>Australia</t>
   </si>
   <si>
+    <t>There are updates.</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
     <t>www.link1.com</t>
   </si>
   <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
     <t>Details of ABC</t>
   </si>
   <si>
@@ -84,6 +87,17 @@
   </si>
   <si>
     <t>Canada</t>
+  </si>
+  <si>
+    <t>There are no updates.</t>
+  </si>
+  <si>
+    <t>1. Topic 1
+2. Topic 2</t>
+  </si>
+  <si>
+    <t>1. Sub-section A
+2. Sub-section B</t>
   </si>
   <si>
     <r>
@@ -146,19 +160,47 @@
     <t>Document 3 &amp; 4 details</t>
   </si>
   <si>
-    <t>1. Topic 1
-2. Topic 2</t>
-  </si>
-  <si>
-    <t>1. Sub-section A
-2. Sub-section B</t>
-  </si>
-  <si>
     <t>1. Updated the date
 2. Updated the document weblink. This links to the pdf document, which shows the updates made in Section V of document 123.</t>
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve">1. Topic 1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>2. Topic 2
+3. Topic 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve">1. Sub-topic a1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>2. Sub-topic b2
+3. Sub-topic c1</t>
+    </r>
   </si>
   <si>
     <r>
@@ -229,42 +271,6 @@
       <t xml:space="preserve">
 2. www.link2.com
 3. www.link3.com</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF000000"/>
-      </rPr>
-      <t xml:space="preserve">1. Topic 1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF000000"/>
-      </rPr>
-      <t>2. Topic 2
-3. Topic 3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF000000"/>
-      </rPr>
-      <t xml:space="preserve">1. Sub-topic a1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF000000"/>
-      </rPr>
-      <t>2. Sub-topic b2
-3. Sub-topic c1</t>
     </r>
   </si>
   <si>
@@ -341,6 +347,9 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -348,9 +357,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -591,19 +597,22 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -611,112 +620,121 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3">
-        <v>45312.0</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4">
+        <v>45312.0</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="6">
         <v>45493.0</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="11">
+      <c r="E3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="11">
         <v>45410.0</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="D4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="J4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="6" t="s">
         <v>28</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="C3"/>
-    <hyperlink r:id="rId3" ref="D3"/>
-    <hyperlink r:id="rId4" ref="C4"/>
+    <hyperlink r:id="rId2" ref="F3"/>
+    <hyperlink r:id="rId3" ref="G3"/>
+    <hyperlink r:id="rId4" ref="F4"/>
   </hyperlinks>
   <drawing r:id="rId5"/>
   <legacyDrawing r:id="rId6"/>

</xml_diff>